<commit_message>
fix: errors in spelling
</commit_message>
<xml_diff>
--- a/templates/export/geofence-visits.xlsx
+++ b/templates/export/geofence-visits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d050092/git/private/Socratec/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E0F1D7-336B-8544-96D7-CBE2705F2535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01E1B1D-3F29-1544-BEC2-95A915A0070A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geofence Visits" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>Report Typ:</t>
   </si>
   <si>
-    <t>Geofence besuche</t>
-  </si>
-  <si>
     <t>Zeitraum:</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>Besuchte Orte</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -529,7 +529,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -538,16 +538,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>